<commit_message>
Update Valkyrie Connection Table.xlsx
</commit_message>
<xml_diff>
--- a/Firmware/RRF/Valkyrie Connection Table.xlsx
+++ b/Firmware/RRF/Valkyrie Connection Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29622"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/Project-Valkyrie/Firmware/RRF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1118" documentId="8_{C788BE8B-89FF-47EE-BC54-747C3D562542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23D64B6B-1C59-4573-B6E5-AF1E28170354}"/>
+  <xr:revisionPtr revIDLastSave="1128" documentId="8_{C788BE8B-89FF-47EE-BC54-747C3D562542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1988216-C740-4E7A-968E-2B05AD06F037}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="16440" xr2:uid="{344B6B93-88E2-4E8A-A19A-9E2625195A37}"/>
   </bookViews>
@@ -1270,7 +1270,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -1592,7 +1592,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1639,7 +1639,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1647,10 +1647,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1820,9 +1816,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1860,7 +1856,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1966,7 +1962,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2108,7 +2104,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2119,20 +2115,20 @@
   <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="28.5" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3455,41 +3451,41 @@
       <c r="A65" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="B65" s="40" t="s">
+      <c r="B65" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="C65" s="40" t="s">
+      <c r="C65" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D65" s="41" t="s">
+      <c r="D65" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="E65" s="41" t="s">
+      <c r="E65" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="F65" s="40"/>
-      <c r="G65" s="42"/>
+      <c r="F65" s="30"/>
+      <c r="G65" s="40"/>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B66" s="40" t="s">
+      <c r="B66" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C66" s="40" t="s">
+      <c r="C66" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="D66" s="41" t="s">
+      <c r="D66" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E66" s="41" t="s">
+      <c r="E66" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="F66" s="40">
-        <v>24</v>
-      </c>
-      <c r="G66" s="42">
+      <c r="F66" s="30">
+        <v>24</v>
+      </c>
+      <c r="G66" s="40">
         <v>110</v>
       </c>
     </row>
@@ -3497,22 +3493,22 @@
       <c r="A67" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B67" s="40" t="s">
+      <c r="B67" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C67" s="40" t="s">
+      <c r="C67" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="D67" s="41" t="s">
+      <c r="D67" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E67" s="41" t="s">
+      <c r="E67" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="F67" s="40">
-        <v>24</v>
-      </c>
-      <c r="G67" s="42">
+      <c r="F67" s="30">
+        <v>24</v>
+      </c>
+      <c r="G67" s="40">
         <v>110</v>
       </c>
     </row>
@@ -3520,39 +3516,39 @@
       <c r="A68" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="B68" s="40" t="s">
+      <c r="B68" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="C68" s="40" t="s">
+      <c r="C68" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="D68" s="41" t="s">
+      <c r="D68" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E68" s="41" t="s">
+      <c r="E68" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="F68" s="40"/>
-      <c r="G68" s="42"/>
+      <c r="F68" s="30"/>
+      <c r="G68" s="40"/>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="43" t="s">
+      <c r="A69" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B69" s="44" t="s">
+      <c r="B69" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="C69" s="44" t="s">
+      <c r="C69" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="D69" s="45" t="s">
+      <c r="D69" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="E69" s="45" t="s">
+      <c r="E69" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="F69" s="44"/>
-      <c r="G69" s="46"/>
+      <c r="F69" s="42"/>
+      <c r="G69" s="44"/>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">

</xml_diff>